<commit_message>
Do zdrojových dokumentů přidána "studie Wach" z prosince 2016 a její doplnění z března 2017
</commit_message>
<xml_diff>
--- a/src/fukce_stavby.xlsx
+++ b/src/fukce_stavby.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="0" windowWidth="18885" windowHeight="8340"/>
+    <workbookView xWindow="4815" yWindow="0" windowWidth="15060" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
   <si>
     <t>Výuka plavání</t>
   </si>
@@ -41,24 +41,6 @@
     <t>Kondiční plavání dospělých</t>
   </si>
   <si>
-    <t>Plavecký trénink sportovců - přípravka</t>
-  </si>
-  <si>
-    <t>Plavecký trénink sportovců - oddíl</t>
-  </si>
-  <si>
-    <t>Plavecký trénink sportovců - centrum vrcholového sportu</t>
-  </si>
-  <si>
-    <t>Vodní pólo</t>
-  </si>
-  <si>
-    <t>Synchronizované plavání</t>
-  </si>
-  <si>
-    <t>Skoky do vody</t>
-  </si>
-  <si>
     <t>Sportovní soutěže</t>
   </si>
   <si>
@@ -95,9 +77,6 @@
     <t>Zdravotní rehabilitace</t>
   </si>
   <si>
-    <t>Výuka přístrojového a nádechového potápění</t>
-  </si>
-  <si>
     <t>Komerční činnost externích subjektů</t>
   </si>
   <si>
@@ -113,15 +92,9 @@
     <t>FUNKCE STAVBY</t>
   </si>
   <si>
-    <t>Plavání kojenců (baby-plavání)</t>
-  </si>
-  <si>
     <t>Sportovní trénink plavání</t>
   </si>
   <si>
-    <t>Plavecký trénink</t>
-  </si>
-  <si>
     <t>Sauna</t>
   </si>
   <si>
@@ -140,9 +113,6 @@
     <t>Rehabilitační cvičení s terapeutem</t>
   </si>
   <si>
-    <t>Vodní sporty a aktivity</t>
-  </si>
-  <si>
     <t>Restaurace "nad vodou"</t>
   </si>
   <si>
@@ -174,6 +144,111 @@
   </si>
   <si>
     <t>Obchod se sportovním zbožím</t>
+  </si>
+  <si>
+    <t>SEKCE</t>
+  </si>
+  <si>
+    <t>VÝUKOVÝ BAZÉN</t>
+  </si>
+  <si>
+    <t>Plavání kojenců a batolat (baby-plavání) 0.5 - 3 roky</t>
+  </si>
+  <si>
+    <t>BAZÉN 50 x 25 m</t>
+  </si>
+  <si>
+    <t>RELAXAČNÍ BAZÉN</t>
+  </si>
+  <si>
+    <t>WELLNESS VÍŘIVKA</t>
+  </si>
+  <si>
+    <t>WELLNESS CHLAD</t>
+  </si>
+  <si>
+    <t>HLEDIŠTĚ</t>
+  </si>
+  <si>
+    <t>VSTUPNÍ LOBBY</t>
+  </si>
+  <si>
+    <t>PARKOVIŠTĚ</t>
+  </si>
+  <si>
+    <t>SERVISNÍ TERMINÁL</t>
+  </si>
+  <si>
+    <t>MOKRÝ BAR</t>
+  </si>
+  <si>
+    <t>RESTAURACE HORNÍ</t>
+  </si>
+  <si>
+    <t>RESTAURACE DOLNÍ</t>
+  </si>
+  <si>
+    <t>ZRCADLOVÝ SÁL</t>
+  </si>
+  <si>
+    <t>KONFERENČNÍ SÁL</t>
+  </si>
+  <si>
+    <t>KANCELÁŘE</t>
+  </si>
+  <si>
+    <t>ÚPRAVNA VODY</t>
+  </si>
+  <si>
+    <t>TECHNICKÉ ZÁZEMÍ</t>
+  </si>
+  <si>
+    <t>SKLAD</t>
+  </si>
+  <si>
+    <t>SCHODIŠTĚ TOBOGÁNU</t>
+  </si>
+  <si>
+    <t>DOJEZDOVÝ BAZÉN TOBO</t>
+  </si>
+  <si>
+    <t>HLUBOKÝ BAZÉN</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Sportovní trénink</t>
+  </si>
+  <si>
+    <t>Plavecká příprava dětí 6-10 let (přípravka)</t>
+  </si>
+  <si>
+    <t>Plavecký trénink dětí 10-18 let (sportovní klub, tzv. "oddíl")</t>
+  </si>
+  <si>
+    <t>Plavecký trénink sportovců 15+ (centrum vrcholového sportu)</t>
+  </si>
+  <si>
+    <t>Vodní pólo - sportovní příprava</t>
+  </si>
+  <si>
+    <t>Synchronizované plavání - sportovní příprava</t>
+  </si>
+  <si>
+    <t>Skoky do vody - sportovní příprava</t>
+  </si>
+  <si>
+    <t>Přístrojové potápění - hobby a profesní příprava</t>
+  </si>
+  <si>
+    <t>Sportovní potápění (plavání s ploutvemi) - sportovní příprava</t>
+  </si>
+  <si>
+    <t>Nádechové potápění (freediving)- sportovní příprava</t>
+  </si>
+  <si>
+    <t>BABY BAZÉNY</t>
   </si>
 </sst>
 </file>
@@ -205,7 +280,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,8 +299,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -285,12 +372,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
@@ -300,28 +396,41 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="15"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="15"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -608,400 +717,560 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F38"/>
+  <dimension ref="A1:AB40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" customWidth="1"/>
-    <col min="6" max="6" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" customWidth="1"/>
+    <col min="12" max="14" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.7109375" customWidth="1"/>
+    <col min="16" max="16" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="3.7109375" customWidth="1"/>
+    <col min="19" max="28" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="2:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="11" t="s">
+    <row r="1" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+    </row>
+    <row r="2" spans="1:28" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q2" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
+      <c r="T2" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="V2" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB2" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="9"/>
+      <c r="E3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="4" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
+      <c r="H5" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="4" t="s">
+      <c r="D6" s="14"/>
+      <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
+      <c r="H6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="4" t="s">
+      <c r="D7" s="14"/>
+      <c r="E7" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D9" s="17"/>
+      <c r="E9" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="17"/>
+      <c r="E10" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="17"/>
+      <c r="E11" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="4" t="s">
+      <c r="D12" s="17"/>
+      <c r="E12" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D13" s="17"/>
+      <c r="E13" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D14" s="17"/>
+      <c r="E14" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D15" s="17"/>
+      <c r="E15" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D16" s="17"/>
+      <c r="E16" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M17" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="O17" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D18" s="18"/>
+      <c r="E18" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O18" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="14"/>
+      <c r="E20" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D21" s="14"/>
+      <c r="E21" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D22" s="14"/>
+      <c r="E22" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D23" s="14"/>
+      <c r="E23" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D24" s="14"/>
+      <c r="E24" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D27" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D28" s="14"/>
+      <c r="E28" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D29" s="14"/>
+      <c r="E29" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="4" t="s">
+      <c r="D30" s="14"/>
+      <c r="E30" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D34" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D35" s="17"/>
+      <c r="E35" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D36" s="17"/>
+      <c r="E36" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D37" s="18"/>
+      <c r="E37" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="4" t="s">
-        <v>40</v>
+      <c r="D38" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="E17:E24"/>
-    <mergeCell ref="E25:E28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="E3:E7"/>
-    <mergeCell ref="E8:E12"/>
-    <mergeCell ref="E13:E16"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D3:D7"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="D8:D18"/>
+    <mergeCell ref="D19:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Pardubice - kapacita, pocet zamestnancu, rozsah rekonstrukce
</commit_message>
<xml_diff>
--- a/src/fukce_stavby.xlsx
+++ b/src/fukce_stavby.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>Výuka plavání</t>
   </si>
@@ -249,6 +249,15 @@
   </si>
   <si>
     <t>BABY BAZÉNY</t>
+  </si>
+  <si>
+    <t>Relaxace  ve vodě</t>
+  </si>
+  <si>
+    <t>SAUNOVÁ KOMORA</t>
+  </si>
+  <si>
+    <t>PARNÍ KOMORA</t>
   </si>
 </sst>
 </file>
@@ -280,7 +289,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -308,6 +317,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFABFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -386,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
@@ -435,6 +468,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -443,6 +494,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFEFABFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -717,13 +773,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB40"/>
+  <dimension ref="A1:AD41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,16 +789,17 @@
     <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" customWidth="1"/>
     <col min="7" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.7109375" customWidth="1"/>
     <col min="12" max="14" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.7109375" customWidth="1"/>
-    <col min="16" max="16" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="3.7109375" customWidth="1"/>
-    <col min="19" max="28" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="3.7109375" customWidth="1"/>
+    <col min="18" max="18" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="3.7109375" customWidth="1"/>
+    <col min="21" max="30" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>21</v>
       </c>
@@ -775,8 +832,10 @@
       <c r="Z1" s="9"/>
       <c r="AA1" s="9"/>
       <c r="AB1" s="9"/>
-    </row>
-    <row r="2" spans="1:28" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+    </row>
+    <row r="2" spans="1:30" ht="123.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>19</v>
       </c>
@@ -793,16 +852,16 @@
         <v>35</v>
       </c>
       <c r="F2" s="15"/>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="J2" s="19" t="s">
         <v>44</v>
       </c>
       <c r="K2" s="11" t="s">
@@ -811,56 +870,62 @@
       <c r="L2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="N2" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="O2" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q2" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="R2" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="S2" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="T2" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="S2" s="10" t="s">
+      <c r="U2" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="V2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="W2" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="X2" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="Y2" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="X2" s="10" t="s">
+      <c r="Z2" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="Y2" s="10" t="s">
+      <c r="AA2" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="Z2" s="10" t="s">
+      <c r="AB2" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="AA2" s="10" t="s">
+      <c r="AC2" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="AB2" s="10" t="s">
+      <c r="AD2" s="10" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -874,7 +939,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -889,7 +954,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -901,7 +966,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -916,7 +981,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -931,7 +996,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -942,7 +1007,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -951,7 +1016,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -960,7 +1025,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -969,7 +1034,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -978,7 +1043,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -987,7 +1052,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -996,7 +1061,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1005,7 +1070,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1014,7 +1079,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1034,11 +1099,11 @@
       <c r="M17" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="O17" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q17" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1046,11 +1111,11 @@
       <c r="E18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="O18" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q18" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1061,7 +1126,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1070,7 +1135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1079,7 +1144,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1088,7 +1153,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1097,7 +1162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1106,7 +1171,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1115,7 +1180,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1124,7 +1189,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1135,7 +1200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1144,7 +1209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1153,7 +1218,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1162,110 +1227,140 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="14"/>
+      <c r="D32" s="17"/>
       <c r="E32" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="5" t="s">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J33" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K33" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="N33" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="R33" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E33" s="4" t="s">
+      <c r="E34" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
-      <c r="D35" s="17"/>
+      <c r="D35" s="16" t="s">
+        <v>17</v>
+      </c>
       <c r="E35" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="17"/>
       <c r="E36" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="18"/>
+      <c r="D37" s="17"/>
       <c r="E37" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="D38" s="18"/>
       <c r="E38" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="14"/>
+      <c r="D39" s="14" t="s">
+        <v>18</v>
+      </c>
       <c r="E39" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="14"/>
       <c r="E40" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="4" t="s">
         <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="D27:D30"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="D34:D37"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="D31:D33"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="D3:D7"/>
     <mergeCell ref="F1:F2"/>

</xml_diff>

<commit_message>
Přidán cash flow diagram provozní roční bilance v základní grafické podobě bez podrobnějšího dělení. Dělení bude přidáno podle vzoru výroční zprávy Mebys Trutnov s.r.o. 2016
</commit_message>
<xml_diff>
--- a/src/fukce_stavby.xlsx
+++ b/src/fukce_stavby.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="0" windowWidth="15060" windowHeight="8280"/>
+    <workbookView xWindow="6420" yWindow="0" windowWidth="15060" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,8 +23,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Zilka, Jan</author>
+  </authors>
+  <commentList>
+    <comment ref="X2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zilka, Jan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Skokanské schody
+Inspirované stavbou, která se nachází v Kopenhagenu</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="99">
   <si>
     <t>Výuka plavání</t>
   </si>
@@ -83,39 +118,18 @@
     <t>Gastronomické služby</t>
   </si>
   <si>
-    <t>ZÁKLADNÍ</t>
-  </si>
-  <si>
-    <t>DOPLŇKOVÉ</t>
-  </si>
-  <si>
     <t>FUNKCE STAVBY</t>
   </si>
   <si>
     <t>Sportovní trénink plavání</t>
   </si>
   <si>
-    <t>Sauna</t>
-  </si>
-  <si>
-    <t>Pára</t>
-  </si>
-  <si>
-    <t>Vířivka</t>
-  </si>
-  <si>
     <t>Relaxační bazén</t>
   </si>
   <si>
-    <t>Tobogán</t>
-  </si>
-  <si>
     <t>Rehabilitační cvičení s terapeutem</t>
   </si>
   <si>
-    <t>Restaurace "nad vodou"</t>
-  </si>
-  <si>
     <t>Mokrý bar "na hladině"</t>
   </si>
   <si>
@@ -137,9 +151,6 @@
     <t>DRUH</t>
   </si>
   <si>
-    <t>VOLITELNÉ</t>
-  </si>
-  <si>
     <t>Kadeřnictví</t>
   </si>
   <si>
@@ -149,27 +160,12 @@
     <t>SEKCE</t>
   </si>
   <si>
-    <t>VÝUKOVÝ BAZÉN</t>
-  </si>
-  <si>
     <t>Plavání kojenců a batolat (baby-plavání) 0.5 - 3 roky</t>
   </si>
   <si>
-    <t>BAZÉN 50 x 25 m</t>
-  </si>
-  <si>
     <t>RELAXAČNÍ BAZÉN</t>
   </si>
   <si>
-    <t>WELLNESS VÍŘIVKA</t>
-  </si>
-  <si>
-    <t>WELLNESS CHLAD</t>
-  </si>
-  <si>
-    <t>HLEDIŠTĚ</t>
-  </si>
-  <si>
     <t>VSTUPNÍ LOBBY</t>
   </si>
   <si>
@@ -182,18 +178,9 @@
     <t>MOKRÝ BAR</t>
   </si>
   <si>
-    <t>RESTAURACE HORNÍ</t>
-  </si>
-  <si>
     <t>RESTAURACE DOLNÍ</t>
   </si>
   <si>
-    <t>ZRCADLOVÝ SÁL</t>
-  </si>
-  <si>
-    <t>KONFERENČNÍ SÁL</t>
-  </si>
-  <si>
     <t>KANCELÁŘE</t>
   </si>
   <si>
@@ -209,9 +196,6 @@
     <t>SCHODIŠTĚ TOBOGÁNU</t>
   </si>
   <si>
-    <t>DOJEZDOVÝ BAZÉN TOBO</t>
-  </si>
-  <si>
     <t>HLUBOKÝ BAZÉN</t>
   </si>
   <si>
@@ -248,23 +232,137 @@
     <t>Nádechové potápění (freediving)- sportovní příprava</t>
   </si>
   <si>
-    <t>BABY BAZÉNY</t>
-  </si>
-  <si>
     <t>Relaxace  ve vodě</t>
   </si>
   <si>
-    <t>SAUNOVÁ KOMORA</t>
-  </si>
-  <si>
     <t>PARNÍ KOMORA</t>
+  </si>
+  <si>
+    <t>SKOKANSKÁ VĚŽ</t>
+  </si>
+  <si>
+    <t>Saunování - finská sauna</t>
+  </si>
+  <si>
+    <t>Relaxace v horké páře</t>
+  </si>
+  <si>
+    <t>Koupání ve vířivce</t>
+  </si>
+  <si>
+    <t>Jízda na tobogánu</t>
+  </si>
+  <si>
+    <t>Lezení nad vodou</t>
+  </si>
+  <si>
+    <t>DOJEZDOVÝ BAZÉN TOBOGÁNU</t>
+  </si>
+  <si>
+    <t>BABY BAZÉN 1</t>
+  </si>
+  <si>
+    <t>BABY BAZÉN 2</t>
+  </si>
+  <si>
+    <t>ČASOMÍRA A VÝSLEDKOVÝ SERVIS</t>
+  </si>
+  <si>
+    <t>ŠATNA SPOLEČNÁ</t>
+  </si>
+  <si>
+    <t>ŠATNA RODIČŮ S DĚTMI</t>
+  </si>
+  <si>
+    <t>SPRCHY MUŽI</t>
+  </si>
+  <si>
+    <t>SPRCHY ŽENY</t>
+  </si>
+  <si>
+    <t>KONFERENČNÍ MÍSTNOST 1</t>
+  </si>
+  <si>
+    <t>KONFERENČNÍ MÍSTNOST 2</t>
+  </si>
+  <si>
+    <t>HOTEL</t>
+  </si>
+  <si>
+    <t>Veřejná restaurace "nad vodou"</t>
+  </si>
+  <si>
+    <t>Služby školní jídelny - obědy</t>
+  </si>
+  <si>
+    <t>Výuka první stupeň ZŠ se sportovním zaměřením</t>
+  </si>
+  <si>
+    <t>Výuka druhý stupeň ZŠ se sportovním zaměřením</t>
+  </si>
+  <si>
+    <t>Výuka</t>
+  </si>
+  <si>
+    <t>VÝUKOVÝ BAZÉN 12.5 x 15m</t>
+  </si>
+  <si>
+    <t>VÍŘIVKA</t>
+  </si>
+  <si>
+    <t>KRYO TERAPIE</t>
+  </si>
+  <si>
+    <t>RESTAURACE HLAVNÍ HORNÍ</t>
+  </si>
+  <si>
+    <t>FINSKÁ SAUNA 1</t>
+  </si>
+  <si>
+    <t>FINSKÁ SAUNA 2</t>
+  </si>
+  <si>
+    <t>CHLADNÉ JEZÍRKO</t>
+  </si>
+  <si>
+    <t>ELEMENTÁRNÍ FUNKCE</t>
+  </si>
+  <si>
+    <t>VOLITELNÉ FUNKCE</t>
+  </si>
+  <si>
+    <t>DOPLŇKOVÉ FUNKCE</t>
+  </si>
+  <si>
+    <t>MÍSTNOST MEDIA / REŽIE</t>
+  </si>
+  <si>
+    <t>MALÁ TĚLOCVIČNA - ZRCADLOVÁ</t>
+  </si>
+  <si>
+    <t>ROZCVIČOVACÍ SÁL - KOBERCOVÝ</t>
+  </si>
+  <si>
+    <t>PLAVECKÝ BAZÉN 50 x 25 m</t>
+  </si>
+  <si>
+    <t>TUBUS TOBOGÁNU</t>
+  </si>
+  <si>
+    <t>SKOKANSKÉ SCHODY S LEZECKOU STĚNOU</t>
+  </si>
+  <si>
+    <t>HLEDIŠTĚ SUCHÉ</t>
+  </si>
+  <si>
+    <t>HLEDIŠTĚ MOKRÉ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,8 +386,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,25 +440,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor rgb="FFEFABFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFEFABFF"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,7 +549,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
@@ -445,46 +575,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -772,14 +909,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AW46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G18" sqref="G18"/>
+      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,23 +929,23 @@
     <col min="6" max="6" width="5" customWidth="1"/>
     <col min="7" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.7109375" customWidth="1"/>
-    <col min="12" max="14" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="3.7109375" customWidth="1"/>
-    <col min="18" max="18" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="3.7109375" customWidth="1"/>
-    <col min="21" max="30" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="3.7109375" customWidth="1"/>
+    <col min="16" max="18" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="27" width="3.7109375" customWidth="1"/>
+    <col min="28" max="49" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="15" t="s">
-        <v>40</v>
+    <row r="1" spans="1:49" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -834,415 +971,537 @@
       <c r="AB1" s="9"/>
       <c r="AC1" s="9"/>
       <c r="AD1" s="9"/>
-    </row>
-    <row r="2" spans="1:30" ht="123.75" x14ac:dyDescent="0.25">
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="9"/>
+      <c r="AR1" s="9"/>
+      <c r="AS1" s="9"/>
+      <c r="AT1" s="9"/>
+      <c r="AU1" s="9"/>
+      <c r="AV1" s="9"/>
+      <c r="AW1" s="9"/>
+    </row>
+    <row r="2" spans="1:49" ht="201.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="K2" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="L2" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="O2" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="P2" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="W2" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="X2" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y2" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC2" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD2" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="22" t="s">
+      <c r="AF2" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG2" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH2" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI2" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ2" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK2" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL2" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM2" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO2" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="AP2" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ2" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="AR2" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="AS2" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="M2" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="N2" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="O2" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q2" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="Y2" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA2" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB2" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC2" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="AD2" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="AT2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="10"/>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="14"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="14"/>
+      <c r="D5" s="13"/>
       <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I5" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="14"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I6" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="14"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="16" t="s">
-        <v>64</v>
+      <c r="D8" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="17"/>
+      <c r="D9" s="15"/>
       <c r="E9" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="17"/>
+      <c r="D10" s="15"/>
       <c r="E10" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="17"/>
+      <c r="D11" s="15"/>
       <c r="E11" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="17"/>
+      <c r="D12" s="15"/>
       <c r="E12" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="17"/>
+      <c r="D13" s="15"/>
       <c r="E13" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="17"/>
+      <c r="D14" s="15"/>
       <c r="E14" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="17"/>
+      <c r="D15" s="15"/>
       <c r="E15" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="W15" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="X15" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y15" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="17"/>
+      <c r="D16" s="15"/>
       <c r="E16" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="17"/>
+      <c r="D17" s="15"/>
       <c r="E17" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="J17" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="M17" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q17" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="L17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y17" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="18"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q18" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y18" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K19" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="14"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K20" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="14"/>
+      <c r="D21" s="13"/>
       <c r="E21" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K21" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="14"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K22" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="14"/>
+      <c r="D23" s="13"/>
       <c r="E23" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K23" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="W23" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="X23" s="11"/>
+      <c r="Y23" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="14"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K24" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="14"/>
+      <c r="D25" s="13"/>
       <c r="E25" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K25" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="14"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K26" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="14" t="s">
+      <c r="D27" s="13" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="14"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="14"/>
+      <c r="D29" s="13"/>
       <c r="E29" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="14"/>
+      <c r="D30" s="13"/>
       <c r="E30" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="16" t="s">
+      <c r="D31" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="17"/>
+      <c r="D32" s="15"/>
       <c r="E32" s="4" t="s">
         <v>4</v>
       </c>
@@ -1251,123 +1510,158 @@
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="18"/>
+      <c r="D33" s="15"/>
       <c r="E33" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I33" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="K33" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="L33" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="M33" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="N33" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="R33" s="12" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="5" t="s">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="N34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q34" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="R34" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="16" t="s">
-        <v>17</v>
-      </c>
       <c r="E35" s="4" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="17"/>
+      <c r="D36" s="14" t="s">
+        <v>17</v>
+      </c>
       <c r="E36" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="17"/>
+      <c r="D37" s="15"/>
       <c r="E37" s="4" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="18"/>
+      <c r="D38" s="15"/>
       <c r="E38" s="4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="D39" s="16"/>
       <c r="E39" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
-      <c r="D40" s="14"/>
+      <c r="D40" s="13" t="s">
+        <v>18</v>
+      </c>
       <c r="E40" s="4" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="14"/>
+      <c r="D41" s="13"/>
       <c r="E41" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E43" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E44" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>80</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E46" s="19" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="D27:D30"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="D31:D33"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="D3:D7"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="D8:D18"/>
     <mergeCell ref="D19:D26"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="D40:D42"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="D3:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Do mapy funkcí přidána rodina funkcí "výuka", která má za cíl popsat potřeby, které má sportovní třída prvního a druhého stupně základní školy
</commit_message>
<xml_diff>
--- a/src/fukce_stavby.xlsx
+++ b/src/fukce_stavby.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="0" windowWidth="15060" windowHeight="8280"/>
+    <workbookView xWindow="8025" yWindow="0" windowWidth="15060" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="100">
   <si>
     <t>Výuka plavání</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Wellness, relaxace</t>
   </si>
   <si>
-    <t>Aktivní odpočinek</t>
-  </si>
-  <si>
     <t>Zdravotní rehabilitace</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>Obchod se sportovním zbožím</t>
   </si>
   <si>
-    <t>SEKCE</t>
-  </si>
-  <si>
     <t>Plavání kojenců a batolat (baby-plavání) 0.5 - 3 roky</t>
   </si>
   <si>
@@ -301,9 +295,6 @@
     <t>Výuka druhý stupeň ZŠ se sportovním zaměřením</t>
   </si>
   <si>
-    <t>Výuka</t>
-  </si>
-  <si>
     <t>VÝUKOVÝ BAZÉN 12.5 x 15m</t>
   </si>
   <si>
@@ -356,6 +347,18 @@
   </si>
   <si>
     <t>HLEDIŠTĚ MOKRÉ</t>
+  </si>
+  <si>
+    <t>Služby senior jídelny  - obědy, večeře</t>
+  </si>
+  <si>
+    <t>DÍLČÍ  ČÁSTI AREÁLU</t>
+  </si>
+  <si>
+    <t>Aktivní odpočinek, cachtání</t>
+  </si>
+  <si>
+    <t>Školní výuka</t>
   </si>
 </sst>
 </file>
@@ -549,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="15"/>
@@ -581,48 +584,51 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -913,17 +919,15 @@
   <dimension ref="A1:AW46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K16" sqref="K16"/>
+      <selection pane="bottomRight" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="3.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="56.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" customWidth="1"/>
@@ -937,15 +941,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:49" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="18" t="s">
-        <v>32</v>
+      <c r="A1" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="21" t="s">
+        <v>97</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -993,140 +997,140 @@
     </row>
     <row r="2" spans="1:49" ht="201.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="21"/>
+      <c r="G2" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="P2" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD2" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE2" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF2" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="AG2" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH2" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI2" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ2" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK2" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL2" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="AM2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO2" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP2" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="AQ2" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F2" s="18"/>
-      <c r="G2" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="J2" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="K2" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="L2" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="O2" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="P2" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q2" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="U2" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="W2" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="X2" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="Y2" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z2" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA2" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AB2" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="AC2" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="AD2" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF2" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="AG2" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="AH2" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="AI2" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ2" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="AK2" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="AL2" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="AM2" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="AN2" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="AO2" s="26" t="s">
+      <c r="AR2" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="AP2" s="26" t="s">
+      <c r="AS2" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="AQ2" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="AR2" s="20" t="s">
+      <c r="AT2" s="10" t="s">
         <v>73</v>
-      </c>
-      <c r="AS2" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="AT2" s="10" t="s">
-        <v>75</v>
       </c>
       <c r="AU2" s="10"/>
       <c r="AV2" s="10"/>
@@ -1136,415 +1140,447 @@
       <c r="A3" s="6"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="25" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>33</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="F3" s="28"/>
       <c r="G3" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="13"/>
+      <c r="D4" s="25"/>
       <c r="E4" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="F4" s="28"/>
       <c r="G4" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="13"/>
+      <c r="D5" s="25"/>
       <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="F5" s="28"/>
       <c r="I5" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="13"/>
+      <c r="D6" s="25"/>
       <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
+      <c r="F6" s="28"/>
       <c r="I6" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="13"/>
+      <c r="D7" s="25"/>
       <c r="E7" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="F7" s="28"/>
       <c r="I7" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="14" t="s">
-        <v>47</v>
+      <c r="D8" s="22" t="s">
+        <v>45</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="F8" s="28"/>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="15"/>
+      <c r="D9" s="23"/>
       <c r="E9" s="4" t="s">
-        <v>48</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F9" s="28"/>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="15"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="4" t="s">
-        <v>49</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F10" s="28"/>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="15"/>
+      <c r="D11" s="23"/>
       <c r="E11" s="4" t="s">
-        <v>50</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="F11" s="28"/>
     </row>
     <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="15"/>
+      <c r="D12" s="23"/>
       <c r="E12" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="15"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="4" t="s">
-        <v>51</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F13" s="28"/>
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="15"/>
+      <c r="D14" s="23"/>
       <c r="E14" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F14" s="28"/>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="15"/>
+      <c r="D15" s="23"/>
       <c r="E15" s="4" t="s">
-        <v>53</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="F15" s="28"/>
       <c r="W15" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="X15" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Y15" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="15"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="4" t="s">
-        <v>55</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="F16" s="28"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="15"/>
+      <c r="D17" s="23"/>
       <c r="E17" s="4" t="s">
-        <v>56</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F17" s="28"/>
       <c r="I17" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q17" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Y17" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="16"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="4" t="s">
-        <v>54</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="F18" s="28"/>
       <c r="K18" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Y18" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="25" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="F19" s="28"/>
       <c r="K19" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="13"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="F20" s="28"/>
       <c r="K20" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="13"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="F21" s="28"/>
       <c r="K21" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="13"/>
+      <c r="D22" s="25"/>
       <c r="E22" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="F22" s="28"/>
       <c r="K22" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="13"/>
+      <c r="D23" s="25"/>
       <c r="E23" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="F23" s="28"/>
       <c r="K23" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="W23" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="X23" s="11"/>
       <c r="Y23" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="13"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="F24" s="28"/>
       <c r="K24" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="13"/>
+      <c r="D25" s="25"/>
       <c r="E25" s="4" t="s">
         <v>12</v>
       </c>
+      <c r="F25" s="28"/>
       <c r="K25" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="13"/>
+      <c r="D26" s="25"/>
       <c r="E26" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="F26" s="28"/>
       <c r="K26" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="13" t="s">
+      <c r="D27" s="25" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="F27" s="28"/>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="13"/>
+      <c r="D28" s="25"/>
       <c r="E28" s="4" t="s">
-        <v>61</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="F28" s="28"/>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="13"/>
+      <c r="D29" s="25"/>
       <c r="E29" s="4" t="s">
-        <v>62</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F29" s="28"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="13"/>
+      <c r="D30" s="25"/>
       <c r="E30" s="4" t="s">
-        <v>21</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F30" s="28"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="14" t="s">
-        <v>15</v>
+      <c r="D31" s="22" t="s">
+        <v>98</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>63</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="F31" s="28"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="15"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="4" t="s">
         <v>4</v>
       </c>
+      <c r="F32" s="28"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="15"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="4" t="s">
-        <v>64</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="F33" s="28"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="16"/>
+      <c r="D34" s="24"/>
       <c r="E34" s="4" t="s">
-        <v>57</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="F34" s="28"/>
       <c r="J34" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K34" s="11"/>
       <c r="L34" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M34" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="N34" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O34" s="11"/>
       <c r="P34" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="Q34" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R34" s="11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
@@ -1552,113 +1588,135 @@
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>22</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F35" s="28"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="14" t="s">
-        <v>17</v>
+      <c r="D36" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="F36" s="28"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="15"/>
+      <c r="D37" s="23"/>
       <c r="E37" s="4" t="s">
-        <v>26</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="F37" s="28"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="15"/>
+      <c r="D38" s="23"/>
       <c r="E38" s="4" t="s">
-        <v>30</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F38" s="28"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="16"/>
+      <c r="D39" s="24"/>
       <c r="E39" s="4" t="s">
-        <v>31</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="F39" s="28"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
-      <c r="D40" s="13" t="s">
-        <v>18</v>
+      <c r="D40" s="25" t="s">
+        <v>17</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>76</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="F40" s="28"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="13"/>
+      <c r="D41" s="25"/>
       <c r="E41" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F41" s="28"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="13"/>
+      <c r="D42" s="25"/>
       <c r="E42" s="4" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F42" s="28"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E43" s="19" t="s">
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43" s="28"/>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="F44" s="28"/>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D45" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="E45" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="F45" s="28"/>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D46" s="25"/>
+      <c r="E46" s="27" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E44" s="19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D45" t="s">
-        <v>80</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="E46" s="19" t="s">
-        <v>79</v>
-      </c>
+      <c r="F46" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="D45:D46"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="D8:D18"/>
     <mergeCell ref="D19:D26"/>
     <mergeCell ref="D27:D30"/>
-    <mergeCell ref="D40:D42"/>
     <mergeCell ref="D36:D39"/>
     <mergeCell ref="D31:D34"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="D3:D7"/>
+    <mergeCell ref="D40:D44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Přidána srovnávací studie Relaxsolution / Radek Steinhaizl
</commit_message>
<xml_diff>
--- a/src/fukce_stavby.xlsx
+++ b/src/fukce_stavby.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\git\plavecky-stadion-prostejov\plavecky-stadion-prostejov\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\home\git-github\plavecky-stadion-prostejov\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A32BDD0-9CEC-49A8-A093-77A2B2A92259}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8025" yWindow="0" windowWidth="15060" windowHeight="8280"/>
+    <workbookView xWindow="9900" yWindow="0" windowWidth="15060" windowHeight="8280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Zilka, Jan</author>
   </authors>
   <commentList>
-    <comment ref="X2" authorId="0" shapeId="0">
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="103">
   <si>
     <t>Výuka plavání</t>
   </si>
@@ -190,9 +191,6 @@
     <t>SCHODIŠTĚ TOBOGÁNU</t>
   </si>
   <si>
-    <t>HLUBOKÝ BAZÉN</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -217,9 +215,6 @@
     <t>Skoky do vody - sportovní příprava</t>
   </si>
   <si>
-    <t>Přístrojové potápění - hobby a profesní příprava</t>
-  </si>
-  <si>
     <t>Sportovní potápění (plavání s ploutvemi) - sportovní příprava</t>
   </si>
   <si>
@@ -247,9 +242,6 @@
     <t>Jízda na tobogánu</t>
   </si>
   <si>
-    <t>Lezení nad vodou</t>
-  </si>
-  <si>
     <t>DOJEZDOVÝ BAZÉN TOBOGÁNU</t>
   </si>
   <si>
@@ -259,9 +251,6 @@
     <t>BABY BAZÉN 2</t>
   </si>
   <si>
-    <t>ČASOMÍRA A VÝSLEDKOVÝ SERVIS</t>
-  </si>
-  <si>
     <t>ŠATNA SPOLEČNÁ</t>
   </si>
   <si>
@@ -355,16 +344,37 @@
     <t>DÍLČÍ  ČÁSTI AREÁLU</t>
   </si>
   <si>
-    <t>Aktivní odpočinek, cachtání</t>
-  </si>
-  <si>
-    <t>Školní výuka</t>
+    <t>Školní výuka plavání</t>
+  </si>
+  <si>
+    <t>Aktivní odpočinek, vodní atrakce</t>
+  </si>
+  <si>
+    <t>HLUBOKÝ BAZÉN (DIVING WELL)</t>
+  </si>
+  <si>
+    <t>MÍSTNOST ČASOMÍRY</t>
+  </si>
+  <si>
+    <t>ŠATNA ŽENY</t>
+  </si>
+  <si>
+    <t>ŠATNA MUŽI</t>
+  </si>
+  <si>
+    <t>Skoky do vody - adventure</t>
+  </si>
+  <si>
+    <t>Lezení nad vodou - adventure</t>
+  </si>
+  <si>
+    <t>Přístrojové potápění - hobby a profesní příprava a testování</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -608,27 +618,27 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -915,14 +925,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AW46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AY47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D48" sqref="D48"/>
+      <selection pane="bottomRight" activeCell="AK19" sqref="AK19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,19 +947,21 @@
     <col min="14" max="15" width="3.7109375" customWidth="1"/>
     <col min="16" max="18" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="27" width="3.7109375" customWidth="1"/>
-    <col min="28" max="49" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="39" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="3.7109375" customWidth="1"/>
+    <col min="42" max="51" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:51" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="21" t="s">
-        <v>97</v>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="24" t="s">
+        <v>93</v>
       </c>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
@@ -994,16 +1006,18 @@
       <c r="AU1" s="9"/>
       <c r="AV1" s="9"/>
       <c r="AW1" s="9"/>
-    </row>
-    <row r="2" spans="1:49" ht="201.75" x14ac:dyDescent="0.25">
+      <c r="AX1" s="9"/>
+      <c r="AY1" s="9"/>
+    </row>
+    <row r="2" spans="1:51" ht="201.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>28</v>
@@ -1011,21 +1025,21 @@
       <c r="E2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="21"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J2" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="19" t="s">
         <v>91</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>95</v>
       </c>
       <c r="L2" s="18" t="s">
         <v>32</v>
@@ -1037,46 +1051,46 @@
         <v>42</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="P2" s="20" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="Q2" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="T2" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="R2" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="T2" s="12" t="s">
-        <v>83</v>
-      </c>
       <c r="U2" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="W2" s="17" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="Y2" s="17" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="Z2" s="10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="AA2" s="10" t="s">
         <v>37</v>
       </c>
       <c r="AB2" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="AC2" s="13" t="s">
         <v>33</v>
@@ -1088,7 +1102,7 @@
         <v>35</v>
       </c>
       <c r="AF2" s="15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="AG2" s="13" t="s">
         <v>38</v>
@@ -1103,620 +1117,651 @@
         <v>41</v>
       </c>
       <c r="AK2" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="AL2" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM2" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="AN2" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AO2" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="AP2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="AQ2" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="AR2" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="AL2" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="AM2" s="10" t="s">
+      <c r="AS2" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT2" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="AN2" s="10" t="s">
+      <c r="AU2" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="AO2" s="19" t="s">
+      <c r="AV2" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AP2" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="AQ2" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="AR2" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="AS2" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="AT2" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="AU2" s="10"/>
-      <c r="AV2" s="10"/>
       <c r="AW2" s="10"/>
-    </row>
-    <row r="3" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="10"/>
+    </row>
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="23" t="s">
         <v>0</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="28"/>
+      <c r="F3" s="22"/>
       <c r="G3" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:49" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="25"/>
+      <c r="D4" s="23"/>
       <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="28"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I4" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="25"/>
+      <c r="D5" s="23"/>
       <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="22"/>
       <c r="I5" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="25"/>
+      <c r="D6" s="23"/>
       <c r="E6" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="28"/>
+      <c r="F6" s="22"/>
       <c r="I6" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
-      <c r="D7" s="25"/>
+      <c r="D7" s="23"/>
       <c r="E7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F7" s="28"/>
+      <c r="F7" s="22"/>
       <c r="I7" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J7" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="22" t="s">
-        <v>45</v>
+      <c r="D8" s="25" t="s">
+        <v>44</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="28"/>
-    </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="23"/>
+      <c r="D9" s="26"/>
       <c r="E9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="28"/>
-    </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="23"/>
+      <c r="D10" s="26"/>
       <c r="E10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="28"/>
-    </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="23"/>
+      <c r="D11" s="26"/>
       <c r="E11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="28"/>
-    </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="23"/>
+      <c r="D12" s="26"/>
       <c r="E12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="28"/>
-    </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+      <c r="F12" s="22"/>
+    </row>
+    <row r="13" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="23"/>
+      <c r="D13" s="26"/>
       <c r="E13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F13" s="28"/>
-    </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="23"/>
+      <c r="D14" s="26"/>
       <c r="E14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="28"/>
-    </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="23"/>
+      <c r="D15" s="26"/>
       <c r="E15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="28"/>
+        <v>50</v>
+      </c>
+      <c r="F15" s="22"/>
       <c r="W15" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X15" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Y15" s="11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="23"/>
+      <c r="D16" s="26"/>
       <c r="E16" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="28"/>
+        <v>51</v>
+      </c>
+      <c r="F16" s="22"/>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="23"/>
+      <c r="D17" s="26"/>
       <c r="E17" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="28"/>
+        <v>52</v>
+      </c>
+      <c r="F17" s="22"/>
       <c r="I17" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L17" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q17" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Y17" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
-      <c r="D18" s="24"/>
+      <c r="D18" s="27"/>
       <c r="E18" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="28"/>
+        <v>102</v>
+      </c>
+      <c r="F18" s="22"/>
       <c r="K18" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Y18" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="23" t="s">
         <v>5</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="28"/>
+      <c r="F19" s="22"/>
       <c r="K19" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
-      <c r="D20" s="25"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="28"/>
+      <c r="F20" s="22"/>
       <c r="K20" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="25"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F21" s="28"/>
+      <c r="F21" s="22"/>
       <c r="K21" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="25"/>
+      <c r="D22" s="23"/>
       <c r="E22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F22" s="28"/>
+      <c r="F22" s="22"/>
       <c r="K22" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
-      <c r="D23" s="25"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="28"/>
+      <c r="F23" s="22"/>
       <c r="K23" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="W23" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="X23" s="11"/>
       <c r="Y23" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="25"/>
+      <c r="D24" s="23"/>
       <c r="E24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="28"/>
+      <c r="F24" s="22"/>
       <c r="K24" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="25"/>
+      <c r="D25" s="23"/>
       <c r="E25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="28"/>
+      <c r="F25" s="22"/>
       <c r="K25" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="25"/>
+      <c r="D26" s="23"/>
       <c r="E26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="28"/>
+      <c r="F26" s="22"/>
       <c r="K26" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="23" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" s="28"/>
+        <v>56</v>
+      </c>
+      <c r="F27" s="22"/>
+      <c r="R27" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="S27" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="T27" s="11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="25"/>
+      <c r="D28" s="23"/>
       <c r="E28" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F28" s="28"/>
+        <v>57</v>
+      </c>
+      <c r="F28" s="22"/>
+      <c r="R28" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="U28" s="11" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="25"/>
+      <c r="D29" s="23"/>
       <c r="E29" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="F29" s="28"/>
+        <v>58</v>
+      </c>
+      <c r="F29" s="22"/>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="25"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F30" s="28"/>
+      <c r="F30" s="22"/>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="22" t="s">
-        <v>98</v>
+      <c r="D31" s="25" t="s">
+        <v>95</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="F31" s="28"/>
+        <v>59</v>
+      </c>
+      <c r="F31" s="22"/>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="23"/>
+      <c r="D32" s="26"/>
       <c r="E32" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="28"/>
+      <c r="F32" s="22"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="23"/>
+      <c r="D33" s="26"/>
       <c r="E33" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F33" s="28"/>
+        <v>101</v>
+      </c>
+      <c r="F33" s="22"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="24"/>
+      <c r="D34" s="26"/>
       <c r="E34" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F34" s="28"/>
-      <c r="J34" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="M34" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="N34" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q34" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="R34" s="11" t="s">
-        <v>44</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="F34" s="22"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="5" t="s">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="22"/>
+      <c r="J35" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="M35" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="N35" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q35" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="R35" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E36" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F35" s="28"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F36" s="28"/>
+      <c r="F36" s="22"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
-      <c r="D37" s="23"/>
+      <c r="D37" s="25" t="s">
+        <v>16</v>
+      </c>
       <c r="E37" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" s="28"/>
+        <v>24</v>
+      </c>
+      <c r="F37" s="22"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
-      <c r="D38" s="23"/>
+      <c r="D38" s="26"/>
       <c r="E38" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F38" s="28"/>
+        <v>25</v>
+      </c>
+      <c r="F38" s="22"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
-      <c r="D39" s="24"/>
+      <c r="D39" s="26"/>
       <c r="E39" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F39" s="28"/>
+        <v>29</v>
+      </c>
+      <c r="F39" s="22"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
-      <c r="D40" s="25" t="s">
-        <v>17</v>
-      </c>
+      <c r="D40" s="27"/>
       <c r="E40" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F40" s="28"/>
+        <v>30</v>
+      </c>
+      <c r="F40" s="22"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="25"/>
+      <c r="D41" s="23" t="s">
+        <v>17</v>
+      </c>
       <c r="E41" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F41" s="28"/>
+        <v>70</v>
+      </c>
+      <c r="F41" s="22"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="25"/>
+      <c r="D42" s="23"/>
       <c r="E42" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F42" s="28"/>
+        <v>23</v>
+      </c>
+      <c r="F42" s="22"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="F43" s="28"/>
+      <c r="D43" s="23"/>
+      <c r="E43" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F43" s="22"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="F44" s="28"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F44" s="22"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D45" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="E45" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="F45" s="28"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45" s="22"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="D46" s="25"/>
-      <c r="E46" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="F46" s="28"/>
+      <c r="D46" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="E46" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="D47" s="23"/>
+      <c r="E47" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="F47" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D46:D47"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="D8:D18"/>
     <mergeCell ref="D19:D26"/>
     <mergeCell ref="D27:D30"/>
-    <mergeCell ref="D36:D39"/>
-    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="D31:D35"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="D3:D7"/>
-    <mergeCell ref="D40:D44"/>
+    <mergeCell ref="D41:D45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>